<commit_message>
Add data, new features, clean up chart
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\king2\Documents\Sam Docs\Python\Data Apps\Preferred Pronounce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB74B164-120D-41A2-B816-AB813EB46183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D87C26F-C9A1-42DC-ACCA-8ABF055D891C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A7134671-C15C-4531-A6D4-3327DA0B4BB1}"/>
   </bookViews>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A52CD65-A2BF-4AC2-8075-EA939B042110}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,12 +441,45 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>45985</v>
+        <v>45967</v>
       </c>
       <c r="B2">
         <v>1000</v>
       </c>
       <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>45975</v>
+      </c>
+      <c r="B3">
+        <v>1000</v>
+      </c>
+      <c r="C3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>45981</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+      <c r="C4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>45985</v>
+      </c>
+      <c r="B5">
+        <v>1000</v>
+      </c>
+      <c r="C5">
         <v>260</v>
       </c>
     </row>

</xml_diff>